<commit_message>
Homework - Incapsulation practice - Task 2
</commit_message>
<xml_diff>
--- a/Lesson 16 - Excel/family_members.xlsx
+++ b/Lesson 16 - Excel/family_members.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,25 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ИТОГО</t>
+        </is>
+      </c>
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>SUM(E2:E6)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>